<commit_message>
updating the LUT files
</commit_message>
<xml_diff>
--- a/Documents/LUT.xlsx
+++ b/Documents/LUT.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t>Bit</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Don’t/invert Pattern</t>
   </si>
   <si>
-    <t>Don’t/insert post pattern</t>
-  </si>
-  <si>
     <t>Don’t/perform buffer swap</t>
   </si>
   <si>
@@ -128,14 +125,68 @@
     <t>Bin. Pattern No.</t>
   </si>
   <si>
-    <t>Trigger Type</t>
+    <t>Trigger Type (00 Internal, 01 Ext. =, 10 Ext. -, 11 No input trigger (continue from previous)</t>
+  </si>
+  <si>
+    <t>Don’t/insert black-fill pattern after current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFAULT.SEQPATLUT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hex </t>
+  </si>
+  <si>
+    <t>Bin</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Hex</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>DEFAULT.SPLASHLUT</t>
+  </si>
+  <si>
+    <t>Order of 24Bit patterns from flash (i.e. next pattern after bufferload)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFAULT.PATTERNCONFIG.NUM_SPLASH </t>
+  </si>
+  <si>
+    <t>DEFAULT.PATTERNCONFIG.PAT_MODE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0 </t>
+  </si>
+  <si>
+    <t>Streaming through vid. Port</t>
+  </si>
+  <si>
+    <t>0x3</t>
+  </si>
+  <si>
+    <t>Streaming through flash memory</t>
+  </si>
+  <si>
+    <t>User guide tab5-1</t>
+  </si>
+  <si>
+    <t>Number of different 24Bit pattern used in pattern seq.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +265,30 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -327,7 +402,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -383,23 +458,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color theme="2"/>
@@ -425,86 +498,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -844,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:AJ42"/>
+  <dimension ref="A1:AJ52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1"/>
+      <selection activeCell="AX40" sqref="AX40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -856,19 +849,24 @@
     <col min="30" max="36" width="4.54296875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="38" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="G4" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="H5" s="6" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.35">
@@ -892,7 +890,7 @@
         <v>6</v>
       </c>
       <c r="AB8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.35">
@@ -923,13 +921,13 @@
         <v>0</v>
       </c>
       <c r="G10" s="14">
+        <v>0</v>
+      </c>
+      <c r="H10" s="15">
         <v>1</v>
       </c>
-      <c r="H10" s="15">
-        <v>0</v>
-      </c>
       <c r="I10" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10" s="17">
         <v>0</v>
@@ -944,7 +942,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10" s="13">
         <v>0</v>
@@ -953,19 +951,19 @@
         <v>0</v>
       </c>
       <c r="S10" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U10" s="18">
         <v>0</v>
       </c>
       <c r="V10" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W10" s="19">
         <v>0</v>
       </c>
       <c r="X10" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z10" s="19">
         <v>1</v>
@@ -974,13 +972,13 @@
         <v>0</v>
       </c>
       <c r="AB10" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC10" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD10" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AE10" s="1" t="str">
         <f>CONCATENATE(A10,B10,C10,D10)</f>
@@ -988,7 +986,7 @@
       </c>
       <c r="AF10" t="str">
         <f>CONCATENATE(F10,G10,H10,I10)</f>
-        <v>0101</v>
+        <v>0010</v>
       </c>
       <c r="AG10" t="str">
         <f>CONCATENATE(K10, L10,M10,N10)</f>
@@ -996,15 +994,15 @@
       </c>
       <c r="AH10" s="1" t="str">
         <f>CONCATENATE(P10,Q10,R10,S10)</f>
-        <v>0001</v>
+        <v>1000</v>
       </c>
       <c r="AI10" t="str">
         <f>CONCATENATE(U10,V10,W10,X10)</f>
-        <v>0101</v>
+        <v>0000</v>
       </c>
       <c r="AJ10" t="str">
         <f>CONCATENATE(Z10,AA10,AB10,AC10)</f>
-        <v>1011</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.35">
@@ -1013,11 +1011,11 @@
       </c>
       <c r="F11" s="1"/>
       <c r="P11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U11" s="10"/>
       <c r="AD11" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AE11" s="11" t="str">
         <f t="shared" ref="AE11:AJ11" si="0">BIN2HEX(AE10)</f>
@@ -1025,7 +1023,7 @@
       </c>
       <c r="AF11" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AG11" s="12" t="str">
         <f t="shared" si="0"/>
@@ -1033,31 +1031,31 @@
       </c>
       <c r="AH11" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="AI11" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AJ11" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>B</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="J13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O13" s="10" t="str">
         <f>CONCATENATE(K10,L10,M10,N10)</f>
         <v>0100</v>
       </c>
       <c r="Y13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AF13" s="10" t="str">
         <f>CONCATENATE(U10,V10,W10,X10,Z10,AA10)</f>
-        <v>010110</v>
+        <v>000010</v>
       </c>
       <c r="AG13" s="8"/>
       <c r="AJ13" s="8"/>
@@ -1075,7 +1073,7 @@
     <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="I15" s="32"/>
       <c r="J15" s="33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K15" s="33"/>
       <c r="L15" s="33"/>
@@ -1094,13 +1092,13 @@
         <v>0</v>
       </c>
       <c r="AH15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.35">
       <c r="I16" s="32"/>
       <c r="J16" s="33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K16" s="33"/>
       <c r="L16" s="33"/>
@@ -1124,10 +1122,10 @@
         <v>2. Pattern</v>
       </c>
     </row>
-    <row r="17" spans="9:34" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.35">
       <c r="I17" s="32"/>
       <c r="J17" s="33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K17" s="33"/>
       <c r="L17" s="33"/>
@@ -1151,10 +1149,10 @@
         <v>3. Pattern</v>
       </c>
     </row>
-    <row r="18" spans="9:34" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.35">
       <c r="I18" s="32"/>
       <c r="J18" s="33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K18" s="33"/>
       <c r="L18" s="33"/>
@@ -1178,10 +1176,10 @@
         <v>4. Pattern</v>
       </c>
     </row>
-    <row r="19" spans="9:34" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.35">
       <c r="I19" s="32"/>
       <c r="J19" s="33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K19" s="33"/>
       <c r="L19" s="33"/>
@@ -1205,10 +1203,10 @@
         <v>5. Pattern</v>
       </c>
     </row>
-    <row r="20" spans="9:34" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.35">
       <c r="I20" s="32"/>
       <c r="J20" s="33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K20" s="33"/>
       <c r="L20" s="33"/>
@@ -1232,10 +1230,10 @@
         <v>6. Pattern</v>
       </c>
     </row>
-    <row r="21" spans="9:34" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
       <c r="I21" s="32"/>
       <c r="J21" s="33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K21" s="33"/>
       <c r="L21" s="33"/>
@@ -1259,10 +1257,10 @@
         <v>7. Pattern</v>
       </c>
     </row>
-    <row r="22" spans="9:34" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.35">
       <c r="I22" s="32"/>
       <c r="J22" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K22" s="33"/>
       <c r="L22" s="33"/>
@@ -1286,19 +1284,19 @@
         <v>8. Pattern</v>
       </c>
     </row>
-    <row r="23" spans="9:34" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
       <c r="I23" s="33"/>
       <c r="J23" s="33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K23" s="33"/>
       <c r="L23" s="33"/>
       <c r="M23" s="33"/>
       <c r="N23" s="35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O23" s="35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P23" s="33"/>
       <c r="AC23">
@@ -1314,7 +1312,7 @@
         <v>9. Pattern</v>
       </c>
     </row>
-    <row r="24" spans="9:34" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.35">
       <c r="I24" s="33"/>
       <c r="J24" s="33"/>
       <c r="K24" s="33"/>
@@ -1336,7 +1334,7 @@
         <v>10. Pattern</v>
       </c>
     </row>
-    <row r="25" spans="9:34" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.35">
       <c r="J25" s="10"/>
       <c r="AC25">
         <f t="shared" si="2"/>
@@ -1351,7 +1349,7 @@
         <v>11. Pattern</v>
       </c>
     </row>
-    <row r="26" spans="9:34" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.35">
       <c r="J26" s="10"/>
       <c r="AC26">
         <f t="shared" si="2"/>
@@ -1366,7 +1364,7 @@
         <v>12. Pattern</v>
       </c>
     </row>
-    <row r="27" spans="9:34" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.35">
       <c r="J27" s="10"/>
       <c r="AC27">
         <f t="shared" si="2"/>
@@ -1381,7 +1379,7 @@
         <v>13. Pattern</v>
       </c>
     </row>
-    <row r="28" spans="9:34" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.35">
       <c r="J28" s="10"/>
       <c r="AC28">
         <f t="shared" si="2"/>
@@ -1396,8 +1394,29 @@
         <v>14. Pattern</v>
       </c>
     </row>
-    <row r="29" spans="9:34" x14ac:dyDescent="0.35">
-      <c r="J29" s="10"/>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" t="s">
+        <v>36</v>
+      </c>
+      <c r="G29" t="s">
+        <v>41</v>
+      </c>
+      <c r="I29" t="s">
+        <v>37</v>
+      </c>
+      <c r="K29" s="10"/>
+      <c r="N29" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>39</v>
+      </c>
       <c r="AC29">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -1411,8 +1430,26 @@
         <v>15. Pattern</v>
       </c>
     </row>
-    <row r="30" spans="9:34" x14ac:dyDescent="0.35">
-      <c r="J30" s="10"/>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="E30">
+        <v>28</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I30" t="str">
+        <f>HEX2BIN(E30)</f>
+        <v>101000</v>
+      </c>
+      <c r="K30" s="10"/>
+      <c r="N30" t="str">
+        <f>TEXT(HEX2DEC(E30),"0")</f>
+        <v>40</v>
+      </c>
+      <c r="Q30">
+        <f>E30</f>
+        <v>28</v>
+      </c>
       <c r="AC30">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -1426,8 +1463,26 @@
         <v>16. Pattern</v>
       </c>
     </row>
-    <row r="31" spans="9:34" x14ac:dyDescent="0.35">
-      <c r="J31" s="10"/>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="C31">
+        <v>42</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I31" t="str">
+        <f>DEC2BIN(C31)</f>
+        <v>101010</v>
+      </c>
+      <c r="K31" s="10"/>
+      <c r="N31">
+        <f>C31</f>
+        <v>42</v>
+      </c>
+      <c r="Q31" t="str">
+        <f>DEC2HEX(C31)</f>
+        <v>2A</v>
+      </c>
       <c r="AC31">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -1441,8 +1496,26 @@
         <v>17. Pattern</v>
       </c>
     </row>
-    <row r="32" spans="9:34" x14ac:dyDescent="0.35">
-      <c r="J32" s="10"/>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>1101</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I32" t="str">
+        <f>HEX2BIN(BIN2HEX(A32))</f>
+        <v>1101</v>
+      </c>
+      <c r="K32" s="10"/>
+      <c r="N32">
+        <f>BIN2DEC(A32)</f>
+        <v>13</v>
+      </c>
+      <c r="Q32" t="str">
+        <f>BIN2HEX(A32)</f>
+        <v>D</v>
+      </c>
       <c r="AC32">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -1456,8 +1529,9 @@
         <v>18. Pattern</v>
       </c>
     </row>
-    <row r="33" spans="10:34" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.35">
       <c r="J33" s="10"/>
+      <c r="N33" s="39"/>
       <c r="AC33">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -1471,7 +1545,7 @@
         <v>19. Pattern</v>
       </c>
     </row>
-    <row r="34" spans="10:34" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.35">
       <c r="AC34">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -1485,7 +1559,7 @@
         <v>20. Pattern</v>
       </c>
     </row>
-    <row r="35" spans="10:34" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.35">
       <c r="AC35">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -1499,7 +1573,7 @@
         <v>21. Pattern</v>
       </c>
     </row>
-    <row r="36" spans="10:34" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.35">
       <c r="AC36">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -1513,7 +1587,7 @@
         <v>22. Pattern</v>
       </c>
     </row>
-    <row r="37" spans="10:34" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.35">
       <c r="AC37">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -1527,7 +1601,7 @@
         <v>23. Pattern</v>
       </c>
     </row>
-    <row r="38" spans="10:34" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.35">
       <c r="AC38">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -1537,10 +1611,13 @@
         <v>10111</v>
       </c>
       <c r="AH38" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="39" spans="10:34" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="37" t="s">
+        <v>42</v>
+      </c>
       <c r="AC39">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -1551,24 +1628,27 @@
       </c>
       <c r="AG39" s="21" t="str">
         <f>IF(I10=0,"w","b")</f>
-        <v>b</v>
+        <v>w</v>
       </c>
       <c r="AH39" s="31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="40" spans="10:34" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:34" x14ac:dyDescent="0.35">
       <c r="AC40" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF40" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="AF40" s="10" t="s">
+      <c r="AH40" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="AH40" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="10:34" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>43</v>
+      </c>
       <c r="AC41">
         <f>BIN2DEC(AF41)</f>
         <v>31</v>
@@ -1578,48 +1658,84 @@
         <v>11111</v>
       </c>
       <c r="AH41" s="31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AC42" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="42" spans="10:34" x14ac:dyDescent="0.35">
-      <c r="AC42" s="10" t="s">
+      <c r="AF42" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="AF42" s="36" t="s">
-        <v>17</v>
-      </c>
       <c r="AH42" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A47" s="40" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>46</v>
+      </c>
+      <c r="D49" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
+        <v>48</v>
+      </c>
+      <c r="D50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="AC41:AH41 AC15:AH39">
-    <cfRule type="expression" dxfId="0" priority="17">
+    <cfRule type="expression" dxfId="5" priority="17">
       <formula>NOT(IF(DEC2BIN(BIN2DEC($AF$13))=$AF15,1,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB40:AH40">
-    <cfRule type="expression" dxfId="5" priority="14">
+    <cfRule type="expression" dxfId="4" priority="14">
       <formula>NOT((AND(IF(BIN2DEC(AB13)&gt;24,1,0),IF(BIN2DEC($AF13)&lt;31,1,0))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB42:AH42">
-    <cfRule type="expression" dxfId="4" priority="12">
+    <cfRule type="expression" dxfId="3" priority="12">
       <formula>NOT((IF(BIN2DEC($AF$13)&gt;31,1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG39">
-    <cfRule type="expression" dxfId="3" priority="23">
+    <cfRule type="expression" dxfId="2" priority="23">
       <formula>IF(I10=1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:O22">
-    <cfRule type="expression" dxfId="2" priority="10">
+    <cfRule type="expression" dxfId="1" priority="10">
       <formula>NOT(IF(DEC2BIN(BIN2DEC($O$13))=$N15,1,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23:O23">
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>NOT(IF(BIN2DEC($O$13)&gt;7,1,0))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>